<commit_message>
The same RelTol and AbsTol for all the three simulation methods.
</commit_message>
<xml_diff>
--- a/doc/benchmark/sim/Summary.xlsx
+++ b/doc/benchmark/sim/Summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\maeda\GitHub\RCGAToolbox\doc\example\PE\testRCGAsimulate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cygwin64\home\maeda\GitHub\RCGAToolbox\doc\benchmark\sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -995,10 +995,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>3.39E-2</v>
+        <v>6.7100000000000007E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>9.5399999999999999E-3</v>
+        <v>2.8900000000000002E-3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -1009,10 +1009,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>1.41E-2</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="D3" s="1">
-        <v>3.3600000000000001E-3</v>
+        <v>9.68E-4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
@@ -1023,10 +1023,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
-        <v>3.8500000000000001E-3</v>
+        <v>2.4099999999999998E-3</v>
       </c>
       <c r="D4" s="1">
-        <v>1.2700000000000001E-3</v>
+        <v>1.6899999999999999E-4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -1037,10 +1037,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>6.2399999999999997E-2</v>
+        <v>9.0300000000000005E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>9.5299999999999996E-4</v>
+        <v>3.15E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -1051,10 +1051,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>3.1600000000000003E-2</v>
+        <v>3.3399999999999999E-2</v>
       </c>
       <c r="D6" s="1">
-        <v>7.2300000000000001E-4</v>
+        <v>1.1800000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
@@ -1065,10 +1065,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>3.2699999999999999E-3</v>
+        <v>2.6199999999999999E-3</v>
       </c>
       <c r="D7" s="1">
-        <v>1.44E-4</v>
+        <v>2.2599999999999999E-4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -1079,10 +1079,10 @@
         <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>4.2900000000000001E-2</v>
+        <v>9.5600000000000004E-2</v>
       </c>
       <c r="D8" s="1">
-        <v>1.7500000000000002E-2</v>
+        <v>1.7899999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -1093,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>2.8199999999999999E-2</v>
+        <v>6.8900000000000003E-2</v>
       </c>
       <c r="D9" s="1">
-        <v>1.5399999999999999E-3</v>
+        <v>1.8799999999999999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -1107,10 +1107,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="1">
-        <v>4.4999999999999997E-3</v>
+        <v>3.8800000000000002E-3</v>
       </c>
       <c r="D10" s="1">
-        <v>2.5700000000000001E-4</v>
+        <v>1.35E-4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -1121,10 +1121,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="1">
-        <v>5.1299999999999998E-2</v>
+        <v>0.115</v>
       </c>
       <c r="D11" s="1">
-        <v>8.83E-4</v>
+        <v>3.0700000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -1135,10 +1135,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="1">
-        <v>3.5499999999999997E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>6.9499999999999998E-4</v>
+        <v>1.97E-3</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
@@ -1149,10 +1149,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1">
-        <v>3.5599999999999998E-3</v>
+        <v>3.0899999999999999E-3</v>
       </c>
       <c r="D13" s="1">
-        <v>1.07E-4</v>
+        <v>1.6000000000000001E-4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -1163,10 +1163,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>2.3400000000000001E-2</v>
+        <v>3.2099999999999997E-2</v>
       </c>
       <c r="D14" s="1">
-        <v>5.1199999999999998E-4</v>
+        <v>8.2400000000000008E-3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -1177,10 +1177,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>1.4200000000000001E-2</v>
+        <v>1.9900000000000001E-2</v>
       </c>
       <c r="D15" s="1">
-        <v>2.6899999999999998E-4</v>
+        <v>6.87E-4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
@@ -1191,10 +1191,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>2.7699999999999999E-3</v>
+        <v>2.2200000000000002E-3</v>
       </c>
       <c r="D16" s="1">
-        <v>7.8100000000000001E-5</v>
+        <v>1.18E-4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -1205,10 +1205,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="1">
-        <v>6.1499999999999999E-2</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="D17" s="1">
-        <v>7.0299999999999996E-4</v>
+        <v>5.0299999999999997E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -1219,10 +1219,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="1">
-        <v>2.0299999999999999E-2</v>
+        <v>1.04E-2</v>
       </c>
       <c r="D18" s="1">
-        <v>5.4900000000000001E-4</v>
+        <v>4.9100000000000001E-4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -1233,10 +1233,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="1">
-        <v>3.2599999999999999E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="D19" s="1">
-        <v>8.14E-5</v>
+        <v>1.21E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>